<commit_message>
L3 Small fix excel, WBT JUnit tests
</commit_message>
<xml_diff>
--- a/Docs/Lab03/Lab03_WBT_TCs_Form.xlsx
+++ b/Docs/Lab03/Lab03_WBT_TCs_Form.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28623"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A28E61CB-36F4-4356-A336-8828E148078F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3ED3188-FF8D-4DFF-8FAC-63974AE78879}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Statement" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="104">
   <si>
     <t>Informaţiile vor fi preluate din fişiere text.</t>
   </si>
@@ -51,9 +51,6 @@
     <t>actual result</t>
   </si>
   <si>
-    <t>..</t>
-  </si>
-  <si>
     <t>Final        TC No.</t>
   </si>
   <si>
@@ -130,9 +127,6 @@
   </si>
   <si>
     <t xml:space="preserve">Lab03. White-box Testing. Code Coverage </t>
-  </si>
-  <si>
-    <t>1, 2,4, 6, 7</t>
   </si>
   <si>
     <t>#TCs run</t>
@@ -225,25 +219,10 @@
     <t>F02_TC02</t>
   </si>
   <si>
-    <t>F02_Cond01 &gt; 100</t>
-  </si>
-  <si>
-    <t>F02_Cond02 &lt; 20</t>
-  </si>
-  <si>
-    <t>F02_Cond03 == i</t>
-  </si>
-  <si>
-    <t>F02_Condnn &lt; n</t>
-  </si>
-  <si>
     <t>F02_P01</t>
   </si>
   <si>
     <t>F02_P02</t>
-  </si>
-  <si>
-    <t>F02_Pnn</t>
   </si>
   <si>
     <t>F01_TC02</t>
@@ -471,7 +450,70 @@
     <t xml:space="preserve">1 -&gt; 2 -F-&gt; 4 -F-&gt; 6 -T-&gt; 7 -F-&gt; 6 -F-&gt; 9 -&gt; 10 </t>
   </si>
   <si>
-    <t xml:space="preserve">1 -&gt; 2 -F-&gt; 4 -F-&gt; 6 -F-&gt; 9 -&gt; 10 </t>
+    <t>type</t>
+  </si>
+  <si>
+    <t>CASH</t>
+  </si>
+  <si>
+    <t>CARD</t>
+  </si>
+  <si>
+    <t>F01_TC03</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>F01_TC04</t>
+  </si>
+  <si>
+    <t>F01_TC05</t>
+  </si>
+  <si>
+    <t>l.size()==0</t>
+  </si>
+  <si>
+    <t>p.hasNext</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,2,4,6,7,8,6,9,10 </t>
+  </si>
+  <si>
+    <t>1,2,3,10</t>
+  </si>
+  <si>
+    <t>1,2,4,5,10</t>
+  </si>
+  <si>
+    <t>1,2,4,6,7,6,7,8,6,7,6,9,10</t>
+  </si>
+  <si>
+    <t>1,2,4,6,7,6,9,10</t>
+  </si>
+  <si>
+    <t>p.getType().equals(type)</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>F02_P04</t>
+  </si>
+  <si>
+    <t>1 -&gt; 2 -F-&gt; 4 -F-&gt; 6 -F-&gt; 9 -&gt; 10 -imposibil</t>
+  </si>
+  <si>
+    <t>F02_TC03</t>
+  </si>
+  <si>
+    <t>F02_TC04</t>
+  </si>
+  <si>
+    <t>F02_TC05</t>
+  </si>
+  <si>
+    <t>l==null</t>
   </si>
 </sst>
 </file>
@@ -590,13 +632,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <i/>
       <sz val="9"/>
@@ -622,6 +657,12 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -701,7 +742,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="33">
+  <borders count="37">
     <border>
       <left/>
       <right/>
@@ -1111,11 +1152,59 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1128,12 +1217,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1158,12 +1241,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1189,8 +1266,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1221,6 +1298,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1230,6 +1317,18 @@
     <xf numFmtId="0" fontId="7" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1239,8 +1338,23 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1252,9 +1366,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1266,14 +1377,53 @@
     <xf numFmtId="0" fontId="13" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1284,27 +1434,12 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="12" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="12" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1317,51 +1452,57 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1373,44 +1514,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1830,49 +1933,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B1" s="9"/>
-      <c r="D1" s="41" t="s">
-        <v>77</v>
-      </c>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="43"/>
+      <c r="B1" s="7"/>
+      <c r="D1" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="45"/>
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B2" s="30" t="s">
-        <v>63</v>
+      <c r="B2" s="26" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O4" s="5"/>
       <c r="P4" s="5"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="N5" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="O5" s="27"/>
-      <c r="P5" s="27"/>
+        <v>26</v>
+      </c>
+      <c r="N5" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="O5" s="23"/>
+      <c r="P5" s="23"/>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="N6" s="23"/>
-      <c r="O6" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="P6" s="23" t="s">
-        <v>57</v>
+      <c r="N6" s="19"/>
+      <c r="O6" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="P6" s="19" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.3">
@@ -1880,13 +1983,13 @@
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="N7" s="23" t="s">
-        <v>58</v>
-      </c>
-      <c r="O7" s="97" t="s">
-        <v>80</v>
-      </c>
-      <c r="P7" s="98">
+      <c r="N7" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="O7" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="P7" s="38">
         <v>234</v>
       </c>
     </row>
@@ -1895,43 +1998,43 @@
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-      <c r="N8" s="23" t="s">
-        <v>59</v>
-      </c>
-      <c r="O8" s="99" t="s">
-        <v>81</v>
-      </c>
-      <c r="P8" s="100">
+      <c r="N8" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="O8" s="39" t="s">
+        <v>74</v>
+      </c>
+      <c r="P8" s="40">
         <v>234</v>
       </c>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="N9" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="O9" s="101" t="s">
-        <v>82</v>
-      </c>
-      <c r="P9" s="100">
+      <c r="N9" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="O9" s="41" t="s">
+        <v>75</v>
+      </c>
+      <c r="P9" s="40">
         <v>234</v>
       </c>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B10" s="96" t="s">
-        <v>79</v>
+      <c r="B10" t="s">
+        <v>72</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B11" s="28"/>
+      <c r="B11" s="24"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -1961,10 +2064,10 @@
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="B1:T21"/>
+  <dimension ref="B1:T24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="R25" sqref="R25"/>
+    <sheetView topLeftCell="A2" zoomScale="80" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="O30" sqref="O30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1977,173 +2080,174 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B1" s="9"/>
-      <c r="D1" s="41" t="s">
+      <c r="B1" s="7"/>
+      <c r="D1" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="45"/>
+    </row>
+    <row r="3" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B3" s="50" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="51"/>
+      <c r="K3" s="52"/>
+    </row>
+    <row r="6" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B6" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="44"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="I6" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="J6" s="44"/>
+      <c r="K6" s="44"/>
+      <c r="L6" s="44"/>
+      <c r="M6" s="44"/>
+      <c r="N6" s="44"/>
+      <c r="O6" s="44"/>
+      <c r="Q6" s="43" t="s">
+        <v>40</v>
+      </c>
+      <c r="R6" s="44"/>
+      <c r="S6" s="44"/>
+      <c r="T6" s="44"/>
+    </row>
+    <row r="8" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="I8" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q8" s="49" t="s">
+        <v>10</v>
+      </c>
+      <c r="R8" s="49"/>
+      <c r="S8" s="49"/>
+      <c r="T8" s="22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="I9" s="25"/>
+      <c r="Q9" s="49" t="s">
+        <v>29</v>
+      </c>
+      <c r="R9" s="49"/>
+      <c r="S9" s="49"/>
+      <c r="T9" s="22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="Q10" s="49" t="s">
+        <v>30</v>
+      </c>
+      <c r="R10" s="49" t="s">
+        <v>9</v>
+      </c>
+      <c r="S10" s="49"/>
+      <c r="T10" s="22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="Q13" s="43" t="s">
+        <v>41</v>
+      </c>
+      <c r="R13" s="44"/>
+      <c r="S13" s="44"/>
+      <c r="T13" s="44"/>
+    </row>
+    <row r="15" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="Q15" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="R15" s="53" t="s">
+        <v>12</v>
+      </c>
+      <c r="S15" s="54"/>
+      <c r="T15" s="55"/>
+    </row>
+    <row r="16" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="Q16" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="R16" s="46" t="s">
+        <v>76</v>
+      </c>
+      <c r="S16" s="47"/>
+      <c r="T16" s="48"/>
+    </row>
+    <row r="17" spans="17:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q17" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="R17" s="46" t="s">
         <v>77</v>
       </c>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="43"/>
-    </row>
-    <row r="3" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B3" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="45"/>
-      <c r="J3" s="45"/>
-      <c r="K3" s="46"/>
-    </row>
-    <row r="6" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B6" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="C6" s="42"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="I6" s="41" t="s">
-        <v>41</v>
-      </c>
-      <c r="J6" s="42"/>
-      <c r="K6" s="42"/>
-      <c r="L6" s="42"/>
-      <c r="M6" s="42"/>
-      <c r="N6" s="42"/>
-      <c r="O6" s="42"/>
-      <c r="Q6" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="R6" s="42"/>
-      <c r="S6" s="42"/>
-      <c r="T6" s="42"/>
-    </row>
-    <row r="8" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="I8" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q8" s="47" t="s">
-        <v>11</v>
-      </c>
-      <c r="R8" s="47"/>
-      <c r="S8" s="47"/>
-      <c r="T8" s="26">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="I9" s="29"/>
-      <c r="Q9" s="47" t="s">
-        <v>30</v>
-      </c>
-      <c r="R9" s="47"/>
-      <c r="S9" s="47"/>
-      <c r="T9" s="26">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="Q10" s="47" t="s">
-        <v>31</v>
-      </c>
-      <c r="R10" s="47" t="s">
-        <v>10</v>
-      </c>
-      <c r="S10" s="47"/>
-      <c r="T10" s="26">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="Q13" s="41" t="s">
-        <v>43</v>
-      </c>
-      <c r="R13" s="42"/>
-      <c r="S13" s="42"/>
-      <c r="T13" s="42"/>
-    </row>
-    <row r="15" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="Q15" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="R15" s="105" t="s">
-        <v>13</v>
-      </c>
-      <c r="S15" s="106"/>
-      <c r="T15" s="107"/>
-    </row>
-    <row r="16" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="Q16" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="R16" s="102" t="s">
-        <v>83</v>
-      </c>
-      <c r="S16" s="103"/>
-      <c r="T16" s="104"/>
-    </row>
-    <row r="17" spans="17:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="Q17" s="27" t="s">
-        <v>51</v>
-      </c>
-      <c r="R17" s="102" t="s">
-        <v>84</v>
-      </c>
-      <c r="S17" s="103"/>
-      <c r="T17" s="104"/>
+      <c r="S17" s="47"/>
+      <c r="T17" s="48"/>
     </row>
     <row r="18" spans="17:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="Q18" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="R18" s="102" t="s">
-        <v>87</v>
-      </c>
-      <c r="S18" s="103"/>
-      <c r="T18" s="104"/>
-    </row>
-    <row r="19" spans="17:20" x14ac:dyDescent="0.3">
-      <c r="Q19" s="27" t="s">
-        <v>85</v>
-      </c>
-      <c r="R19" s="102" t="s">
-        <v>88</v>
-      </c>
-      <c r="S19" s="103"/>
-      <c r="T19" s="104"/>
+      <c r="Q18" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="R18" s="46" t="s">
+        <v>81</v>
+      </c>
+      <c r="S18" s="47"/>
+      <c r="T18" s="48"/>
+    </row>
+    <row r="19" spans="17:20" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q19" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="R19" s="46" t="s">
+        <v>80</v>
+      </c>
+      <c r="S19" s="47"/>
+      <c r="T19" s="48"/>
     </row>
     <row r="20" spans="17:20" x14ac:dyDescent="0.3">
-      <c r="Q20" s="27" t="s">
-        <v>86</v>
-      </c>
-      <c r="R20" s="102" t="s">
-        <v>89</v>
-      </c>
-      <c r="S20" s="103"/>
-      <c r="T20" s="104"/>
+      <c r="Q20" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="R20" s="46" t="s">
+        <v>99</v>
+      </c>
+      <c r="S20" s="47"/>
+      <c r="T20" s="48"/>
     </row>
     <row r="21" spans="17:20" x14ac:dyDescent="0.3">
-      <c r="Q21" s="27"/>
-      <c r="R21" s="102"/>
-      <c r="S21" s="103"/>
-      <c r="T21" s="104"/>
+      <c r="Q21" s="23"/>
+      <c r="R21" s="46"/>
+      <c r="S21" s="47"/>
+      <c r="T21" s="48"/>
+    </row>
+    <row r="24" spans="17:20" x14ac:dyDescent="0.3">
+      <c r="R24" s="46"/>
+      <c r="S24" s="47"/>
+      <c r="T24" s="48"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="R19:T19"/>
-    <mergeCell ref="R17:T17"/>
-    <mergeCell ref="R15:T15"/>
-    <mergeCell ref="R21:T21"/>
-    <mergeCell ref="R20:T20"/>
+  <mergeCells count="17">
     <mergeCell ref="R18:T18"/>
+    <mergeCell ref="R24:T24"/>
     <mergeCell ref="Q9:S9"/>
     <mergeCell ref="R16:T16"/>
     <mergeCell ref="Q13:T13"/>
@@ -2154,8 +2258,13 @@
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="I6:O6"/>
     <mergeCell ref="Q6:T6"/>
+    <mergeCell ref="R19:T19"/>
+    <mergeCell ref="R17:T17"/>
+    <mergeCell ref="R15:T15"/>
+    <mergeCell ref="R21:T21"/>
+    <mergeCell ref="R20:T20"/>
   </mergeCells>
-  <phoneticPr fontId="19" type="noConversion"/>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -2170,7 +2279,7 @@
   <dimension ref="B1:AB16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2182,10 +2291,10 @@
     <col min="7" max="7" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.21875" customWidth="1"/>
     <col min="9" max="9" width="9.21875" customWidth="1"/>
-    <col min="10" max="10" width="14.6640625" customWidth="1"/>
-    <col min="11" max="11" width="6.109375" customWidth="1"/>
-    <col min="12" max="12" width="6.44140625" customWidth="1"/>
-    <col min="13" max="13" width="5" customWidth="1"/>
+    <col min="10" max="10" width="11.44140625" customWidth="1"/>
+    <col min="11" max="11" width="10.6640625" customWidth="1"/>
+    <col min="12" max="12" width="10.109375" customWidth="1"/>
+    <col min="13" max="13" width="15.21875" customWidth="1"/>
     <col min="15" max="15" width="11.77734375" customWidth="1"/>
     <col min="16" max="16" width="8.77734375" customWidth="1"/>
     <col min="17" max="17" width="8.88671875" customWidth="1"/>
@@ -2199,449 +2308,486 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:28" x14ac:dyDescent="0.3">
-      <c r="B1" s="9"/>
-      <c r="D1" s="41" t="s">
-        <v>77</v>
-      </c>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="43"/>
+      <c r="B1" s="7"/>
+      <c r="D1" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="45"/>
     </row>
     <row r="3" spans="2:28" x14ac:dyDescent="0.3">
-      <c r="B3" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="46"/>
+      <c r="B3" s="50" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="52"/>
     </row>
     <row r="5" spans="2:28" x14ac:dyDescent="0.3">
-      <c r="B5" s="8"/>
+      <c r="B5" s="6"/>
     </row>
     <row r="6" spans="2:28" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B6" s="48" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="48" t="s">
+      <c r="B6" s="59" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="59" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="49" t="s">
+      <c r="E6" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="48" t="s">
+      <c r="F6" s="59"/>
+      <c r="G6" s="59"/>
+      <c r="H6" s="59"/>
+      <c r="I6" s="59"/>
+      <c r="J6" s="59"/>
+      <c r="K6" s="59"/>
+      <c r="L6" s="59"/>
+      <c r="M6" s="59"/>
+      <c r="N6" s="59"/>
+      <c r="O6" s="59"/>
+      <c r="P6" s="59"/>
+      <c r="Q6" s="59"/>
+      <c r="R6" s="59"/>
+      <c r="S6" s="59"/>
+      <c r="T6" s="59"/>
+      <c r="U6" s="59"/>
+      <c r="V6" s="59"/>
+      <c r="W6" s="59"/>
+      <c r="X6" s="59"/>
+      <c r="Y6" s="59"/>
+      <c r="Z6" s="59"/>
+      <c r="AA6" s="59"/>
+      <c r="AB6" s="59"/>
+    </row>
+    <row r="7" spans="2:28" ht="15.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="59"/>
+      <c r="C7" s="59"/>
+      <c r="D7" s="61"/>
+      <c r="E7" s="69" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="66" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" s="70"/>
+      <c r="H7" s="70"/>
+      <c r="I7" s="70"/>
+      <c r="J7" s="70"/>
+      <c r="K7" s="70"/>
+      <c r="L7" s="70"/>
+      <c r="M7" s="67"/>
+      <c r="N7" s="56" t="s">
+        <v>55</v>
+      </c>
+      <c r="O7" s="57"/>
+      <c r="P7" s="57"/>
+      <c r="Q7" s="58"/>
+      <c r="R7" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="48"/>
-      <c r="G6" s="48"/>
-      <c r="H6" s="48"/>
-      <c r="I6" s="48"/>
-      <c r="J6" s="48"/>
-      <c r="K6" s="48"/>
-      <c r="L6" s="48"/>
-      <c r="M6" s="48"/>
-      <c r="N6" s="48"/>
-      <c r="O6" s="48"/>
-      <c r="P6" s="48"/>
-      <c r="Q6" s="48"/>
-      <c r="R6" s="48"/>
-      <c r="S6" s="48"/>
-      <c r="T6" s="48"/>
-      <c r="U6" s="48"/>
-      <c r="V6" s="48"/>
-      <c r="W6" s="48"/>
-      <c r="X6" s="48"/>
-      <c r="Y6" s="48"/>
-      <c r="Z6" s="48"/>
-      <c r="AA6" s="48"/>
-      <c r="AB6" s="48"/>
-    </row>
-    <row r="7" spans="2:28" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B7" s="48"/>
-      <c r="C7" s="48"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="56" t="s">
+      <c r="S7" s="62"/>
+      <c r="T7" s="62"/>
+      <c r="U7" s="62"/>
+      <c r="V7" s="62"/>
+      <c r="W7" s="62"/>
+      <c r="X7" s="62"/>
+    </row>
+    <row r="8" spans="2:28" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="59"/>
+      <c r="C8" s="63" t="s">
+        <v>82</v>
+      </c>
+      <c r="D8" s="63" t="s">
+        <v>86</v>
+      </c>
+      <c r="E8" s="69"/>
+      <c r="F8" s="65" t="s">
+        <v>103</v>
+      </c>
+      <c r="G8" s="65"/>
+      <c r="H8" s="65" t="s">
+        <v>89</v>
+      </c>
+      <c r="I8" s="65"/>
+      <c r="J8" s="65" t="s">
+        <v>90</v>
+      </c>
+      <c r="K8" s="65"/>
+      <c r="L8" s="66" t="s">
+        <v>96</v>
+      </c>
+      <c r="M8" s="67"/>
+      <c r="N8" s="68" t="s">
+        <v>44</v>
+      </c>
+      <c r="O8" s="68" t="s">
+        <v>45</v>
+      </c>
+      <c r="P8" s="68" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q8" s="68" t="s">
+        <v>98</v>
+      </c>
+      <c r="R8" s="62">
+        <v>0</v>
+      </c>
+      <c r="S8" s="62">
+        <v>1</v>
+      </c>
+      <c r="T8" s="62">
+        <v>2</v>
+      </c>
+      <c r="U8" s="62" t="s">
+        <v>17</v>
+      </c>
+      <c r="V8" s="62" t="s">
+        <v>18</v>
+      </c>
+      <c r="W8" s="62" t="s">
+        <v>19</v>
+      </c>
+      <c r="X8" s="62" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="2:28" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B9" s="59"/>
+      <c r="C9" s="64"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="69"/>
+      <c r="F9" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L9" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="M9" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="N9" s="68"/>
+      <c r="O9" s="68"/>
+      <c r="P9" s="68"/>
+      <c r="Q9" s="68"/>
+      <c r="R9" s="62"/>
+      <c r="S9" s="62"/>
+      <c r="T9" s="62"/>
+      <c r="U9" s="62"/>
+      <c r="V9" s="62"/>
+      <c r="W9" s="62"/>
+      <c r="X9" s="62"/>
+    </row>
+    <row r="10" spans="2:28" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B10" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D10" s="10">
         <v>28</v>
       </c>
-      <c r="F7" s="55" t="s">
-        <v>29</v>
-      </c>
-      <c r="G7" s="55"/>
-      <c r="H7" s="55"/>
-      <c r="I7" s="55"/>
-      <c r="J7" s="55"/>
-      <c r="K7" s="55"/>
-      <c r="L7" s="55"/>
-      <c r="M7" s="55"/>
-      <c r="N7" s="55"/>
-      <c r="O7" s="55"/>
-      <c r="P7" s="52" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q7" s="52"/>
-      <c r="R7" s="52"/>
-      <c r="S7" s="52"/>
-      <c r="T7" s="52"/>
-      <c r="U7" s="52"/>
-      <c r="V7" s="51" t="s">
-        <v>17</v>
-      </c>
-      <c r="W7" s="51"/>
-      <c r="X7" s="51"/>
-      <c r="Y7" s="51"/>
-      <c r="Z7" s="51"/>
-      <c r="AA7" s="51"/>
-      <c r="AB7" s="51"/>
-    </row>
-    <row r="8" spans="2:28" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="48"/>
-      <c r="C8" s="53" t="s">
+      <c r="E10" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="J10" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="K10" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="L10" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="M10" s="12"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
+      <c r="P10" s="13"/>
+      <c r="Q10" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="R10" s="14"/>
+      <c r="S10" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="T10" s="14"/>
+      <c r="U10" s="14"/>
+      <c r="V10" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="W10" s="14"/>
+      <c r="X10" s="14"/>
+    </row>
+    <row r="11" spans="2:28" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B11" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D11" s="10">
+        <v>0</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="P11" s="13"/>
+      <c r="Q11" s="13"/>
+      <c r="R11" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="S11" s="14"/>
+      <c r="T11" s="14"/>
+      <c r="U11" s="14"/>
+      <c r="V11" s="14"/>
+      <c r="W11" s="14"/>
+      <c r="X11" s="14"/>
+    </row>
+    <row r="12" spans="2:28" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B12" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D12" s="42">
+        <v>0</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="12"/>
+      <c r="N12" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="O12" s="13"/>
+      <c r="P12" s="13"/>
+      <c r="Q12" s="13"/>
+      <c r="R12" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="S12" s="14"/>
+      <c r="T12" s="14"/>
+      <c r="U12" s="14"/>
+      <c r="V12" s="14"/>
+      <c r="W12" s="14"/>
+      <c r="X12" s="14"/>
+    </row>
+    <row r="13" spans="2:28" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="B13" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D13" s="10">
+        <v>28</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="J13" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="K13" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="L13" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="M13" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="N13" s="13"/>
+      <c r="O13" s="13"/>
+      <c r="P13" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q13" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="R13" s="14"/>
+      <c r="S13" s="14"/>
+      <c r="T13" s="14"/>
+      <c r="U13" s="14"/>
+      <c r="V13" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="W13" s="14"/>
+      <c r="X13" s="14"/>
+    </row>
+    <row r="14" spans="2:28" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B14" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D14" s="10">
+        <v>0</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="J14" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="K14" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="L14" s="12"/>
+      <c r="M14" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="N14" s="13"/>
+      <c r="O14" s="13"/>
+      <c r="P14" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q14" s="13"/>
+      <c r="R14" s="14"/>
+      <c r="S14" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="T14" s="14"/>
+      <c r="U14" s="14"/>
+      <c r="V14" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="W14" s="14"/>
+      <c r="X14" s="14"/>
+    </row>
+    <row r="15" spans="2:28" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B15" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="53" t="s">
-        <v>1</v>
-      </c>
-      <c r="E8" s="56"/>
-      <c r="F8" s="55" t="s">
-        <v>46</v>
-      </c>
-      <c r="G8" s="55"/>
-      <c r="H8" s="55" t="s">
-        <v>47</v>
-      </c>
-      <c r="I8" s="55"/>
-      <c r="J8" s="55" t="s">
-        <v>48</v>
-      </c>
-      <c r="K8" s="55"/>
-      <c r="L8" s="55" t="s">
-        <v>1</v>
-      </c>
-      <c r="M8" s="55"/>
-      <c r="N8" s="55" t="s">
-        <v>49</v>
-      </c>
-      <c r="O8" s="55"/>
-      <c r="P8" s="52" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q8" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="R8" s="52" t="s">
-        <v>1</v>
-      </c>
-      <c r="S8" s="52" t="s">
-        <v>1</v>
-      </c>
-      <c r="T8" s="52" t="s">
-        <v>1</v>
-      </c>
-      <c r="U8" s="52" t="s">
-        <v>52</v>
-      </c>
-      <c r="V8" s="51">
-        <v>0</v>
-      </c>
-      <c r="W8" s="51">
-        <v>1</v>
-      </c>
-      <c r="X8" s="51">
-        <v>2</v>
-      </c>
-      <c r="Y8" s="51" t="s">
-        <v>18</v>
-      </c>
-      <c r="Z8" s="51" t="s">
-        <v>19</v>
-      </c>
-      <c r="AA8" s="51" t="s">
-        <v>20</v>
-      </c>
-      <c r="AB8" s="51" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="2:28" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B9" s="48"/>
-      <c r="C9" s="54"/>
-      <c r="D9" s="54"/>
-      <c r="E9" s="56"/>
-      <c r="F9" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="H9" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="I9" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="J9" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="K9" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="L9" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="M9" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="N9" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="O9" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="P9" s="52"/>
-      <c r="Q9" s="52"/>
-      <c r="R9" s="52"/>
-      <c r="S9" s="52"/>
-      <c r="T9" s="52"/>
-      <c r="U9" s="52"/>
-      <c r="V9" s="51"/>
-      <c r="W9" s="51"/>
-      <c r="X9" s="51"/>
-      <c r="Y9" s="51"/>
-      <c r="Z9" s="51"/>
-      <c r="AA9" s="51"/>
-      <c r="AB9" s="51"/>
-    </row>
-    <row r="10" spans="2:28" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B10" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="14"/>
-      <c r="N10" s="14"/>
-      <c r="O10" s="14"/>
-      <c r="P10" s="15"/>
-      <c r="Q10" s="15"/>
-      <c r="R10" s="15"/>
-      <c r="S10" s="15"/>
-      <c r="T10" s="15"/>
-      <c r="U10" s="15"/>
-      <c r="V10" s="16"/>
-      <c r="W10" s="16"/>
-      <c r="X10" s="16"/>
-      <c r="Y10" s="16"/>
-      <c r="Z10" s="16"/>
-      <c r="AA10" s="16"/>
-      <c r="AB10" s="16"/>
-    </row>
-    <row r="11" spans="2:28" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B11" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="E11" s="13"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="14"/>
-      <c r="N11" s="14"/>
-      <c r="O11" s="14"/>
-      <c r="P11" s="15"/>
-      <c r="Q11" s="15"/>
-      <c r="R11" s="15"/>
-      <c r="S11" s="15"/>
-      <c r="T11" s="15"/>
-      <c r="U11" s="15"/>
-      <c r="V11" s="16"/>
-      <c r="W11" s="16"/>
-      <c r="X11" s="16"/>
-      <c r="Y11" s="16"/>
-      <c r="Z11" s="16"/>
-      <c r="AA11" s="16"/>
-      <c r="AB11" s="16"/>
-    </row>
-    <row r="12" spans="2:28" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B12" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C12" s="17"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="14"/>
-      <c r="O12" s="14"/>
-      <c r="P12" s="15"/>
-      <c r="Q12" s="15"/>
-      <c r="R12" s="15"/>
-      <c r="S12" s="15"/>
-      <c r="T12" s="15"/>
-      <c r="U12" s="15"/>
-      <c r="V12" s="16"/>
-      <c r="W12" s="16"/>
-      <c r="X12" s="16"/>
-      <c r="Y12" s="16"/>
-      <c r="Z12" s="16"/>
-      <c r="AA12" s="16"/>
-      <c r="AB12" s="16"/>
-    </row>
-    <row r="13" spans="2:28" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B13" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" s="11"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="14"/>
-      <c r="O13" s="14"/>
-      <c r="P13" s="15"/>
-      <c r="Q13" s="15"/>
-      <c r="R13" s="15"/>
-      <c r="S13" s="15"/>
-      <c r="T13" s="15"/>
-      <c r="U13" s="15"/>
-      <c r="V13" s="16"/>
-      <c r="W13" s="16"/>
-      <c r="X13" s="16"/>
-      <c r="Y13" s="16"/>
-      <c r="Z13" s="16"/>
-      <c r="AA13" s="16"/>
-      <c r="AB13" s="16"/>
-    </row>
-    <row r="14" spans="2:28" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B14" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" s="11"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="14"/>
-      <c r="O14" s="14"/>
-      <c r="P14" s="15"/>
-      <c r="Q14" s="15"/>
-      <c r="R14" s="15"/>
-      <c r="S14" s="15"/>
-      <c r="T14" s="15"/>
-      <c r="U14" s="15"/>
-      <c r="V14" s="16"/>
-      <c r="W14" s="16"/>
-      <c r="X14" s="16"/>
-      <c r="Y14" s="16"/>
-      <c r="Z14" s="16"/>
-      <c r="AA14" s="16"/>
-      <c r="AB14" s="16"/>
-    </row>
-    <row r="15" spans="2:28" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B15" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" s="11"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="14"/>
-      <c r="N15" s="14"/>
-      <c r="O15" s="14"/>
-      <c r="P15" s="15"/>
-      <c r="Q15" s="15"/>
-      <c r="R15" s="15"/>
-      <c r="S15" s="15"/>
-      <c r="T15" s="15"/>
-      <c r="U15" s="15"/>
-      <c r="V15" s="16"/>
-      <c r="W15" s="16"/>
-      <c r="X15" s="16"/>
-      <c r="Y15" s="16"/>
-      <c r="Z15" s="16"/>
-      <c r="AA15" s="16"/>
-      <c r="AB15" s="16"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="12"/>
+      <c r="N15" s="13"/>
+      <c r="O15" s="13"/>
+      <c r="P15" s="13"/>
+      <c r="Q15" s="13"/>
+      <c r="R15" s="14"/>
+      <c r="S15" s="14"/>
+      <c r="T15" s="14"/>
+      <c r="U15" s="14"/>
+      <c r="V15" s="14"/>
+      <c r="W15" s="14"/>
+      <c r="X15" s="14"/>
     </row>
     <row r="16" spans="2:28" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B16" s="19"/>
+      <c r="B16" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="30">
+  <mergeCells count="27">
     <mergeCell ref="C8:C9"/>
-    <mergeCell ref="N8:O8"/>
     <mergeCell ref="E7:E9"/>
-    <mergeCell ref="F7:O7"/>
-    <mergeCell ref="P7:U7"/>
-    <mergeCell ref="AB8:AB9"/>
+    <mergeCell ref="F7:M7"/>
     <mergeCell ref="H8:I8"/>
     <mergeCell ref="J8:K8"/>
     <mergeCell ref="L8:M8"/>
-    <mergeCell ref="V8:V9"/>
+    <mergeCell ref="R8:R9"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="O8:O9"/>
     <mergeCell ref="P8:P9"/>
     <mergeCell ref="Q8:Q9"/>
-    <mergeCell ref="R8:R9"/>
-    <mergeCell ref="S8:S9"/>
+    <mergeCell ref="N7:Q7"/>
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="B6:B9"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="E6:AB6"/>
-    <mergeCell ref="Z8:Z9"/>
-    <mergeCell ref="AA8:AA9"/>
-    <mergeCell ref="U8:U9"/>
+    <mergeCell ref="V8:V9"/>
+    <mergeCell ref="W8:W9"/>
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="F8:G8"/>
-    <mergeCell ref="W8:W9"/>
+    <mergeCell ref="S8:S9"/>
+    <mergeCell ref="T8:T9"/>
+    <mergeCell ref="U8:U9"/>
+    <mergeCell ref="R7:X7"/>
     <mergeCell ref="X8:X9"/>
-    <mergeCell ref="Y8:Y9"/>
-    <mergeCell ref="T8:T9"/>
-    <mergeCell ref="V7:AB7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2655,8 +2801,8 @@
   </sheetPr>
   <dimension ref="B1:N16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14:G15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2675,72 +2821,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B1" s="9"/>
-      <c r="D1" s="41" t="s">
-        <v>77</v>
-      </c>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="43"/>
+      <c r="B1" s="7"/>
+      <c r="D1" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="45"/>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B3" s="59" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" s="59"/>
-      <c r="D3" s="59"/>
-      <c r="E3" s="59"/>
-      <c r="F3" s="59"/>
-      <c r="G3" s="59"/>
-      <c r="H3" s="59"/>
-      <c r="I3" s="59"/>
-      <c r="J3" s="59"/>
-      <c r="K3" s="59"/>
-      <c r="L3" s="59"/>
+      <c r="B3" s="82" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="82"/>
+      <c r="D3" s="82"/>
+      <c r="E3" s="82"/>
+      <c r="F3" s="82"/>
+      <c r="G3" s="82"/>
+      <c r="H3" s="82"/>
+      <c r="I3" s="82"/>
+      <c r="J3" s="82"/>
+      <c r="K3" s="82"/>
+      <c r="L3" s="82"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B4" s="60" t="s">
+      <c r="B4" s="83" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="87" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="69" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="71" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="62" t="s">
+      <c r="D4" s="89" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="68"/>
-      <c r="G4" s="68"/>
-      <c r="H4" s="68"/>
-      <c r="I4" s="68"/>
-      <c r="J4" s="63"/>
-      <c r="K4" s="62" t="s">
+      <c r="F4" s="80"/>
+      <c r="G4" s="80"/>
+      <c r="H4" s="80"/>
+      <c r="I4" s="80"/>
+      <c r="J4" s="81"/>
+      <c r="K4" s="79" t="s">
         <v>3</v>
       </c>
-      <c r="L4" s="63"/>
+      <c r="L4" s="81"/>
     </row>
     <row r="5" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="61"/>
-      <c r="C5" s="70"/>
-      <c r="D5" s="72"/>
-      <c r="E5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I5" s="64" t="s">
-        <v>1</v>
-      </c>
-      <c r="J5" s="65"/>
+      <c r="B5" s="84"/>
+      <c r="C5" s="88"/>
+      <c r="D5" s="90"/>
+      <c r="E5" s="73" t="s">
+        <v>82</v>
+      </c>
+      <c r="F5" s="74"/>
+      <c r="G5" s="74"/>
+      <c r="H5" s="74"/>
+      <c r="I5" s="74"/>
+      <c r="J5" s="75"/>
       <c r="K5" s="2" t="s">
         <v>4</v>
       </c>
@@ -2749,160 +2887,120 @@
       </c>
     </row>
     <row r="6" spans="2:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="20">
+      <c r="B6" s="16">
         <v>9</v>
       </c>
-      <c r="C6" s="66" t="s">
-        <v>38</v>
+      <c r="C6" s="85" t="s">
+        <v>36</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E6" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="F6" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="G6" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="H6" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="I6" s="73" t="s">
-        <v>1</v>
-      </c>
-      <c r="J6" s="74"/>
-      <c r="K6" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="L6" s="20" t="s">
-        <v>1</v>
+        <v>42</v>
+      </c>
+      <c r="E6" s="76" t="s">
+        <v>83</v>
+      </c>
+      <c r="F6" s="77"/>
+      <c r="G6" s="77"/>
+      <c r="H6" s="77"/>
+      <c r="I6" s="77"/>
+      <c r="J6" s="78"/>
+      <c r="K6" s="17">
+        <v>28</v>
+      </c>
+      <c r="L6" s="16">
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B7" s="20">
+      <c r="B7" s="16">
         <v>10</v>
       </c>
-      <c r="C7" s="66"/>
+      <c r="C7" s="85"/>
       <c r="D7" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E7" s="20">
-        <v>5</v>
-      </c>
-      <c r="F7" s="20">
-        <v>6</v>
-      </c>
-      <c r="G7" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="H7" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="I7" s="62" t="s">
-        <v>1</v>
-      </c>
-      <c r="J7" s="63"/>
-      <c r="K7" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="L7" s="20" t="s">
-        <v>1</v>
+        <v>43</v>
+      </c>
+      <c r="E7" s="79" t="s">
+        <v>83</v>
+      </c>
+      <c r="F7" s="80"/>
+      <c r="G7" s="80"/>
+      <c r="H7" s="80"/>
+      <c r="I7" s="80"/>
+      <c r="J7" s="81"/>
+      <c r="K7" s="16">
+        <v>0</v>
+      </c>
+      <c r="L7" s="16">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B8" s="20">
+      <c r="B8" s="16">
         <v>11</v>
       </c>
-      <c r="C8" s="66"/>
-      <c r="D8" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E8" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="F8" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="G8" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="H8" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="I8" s="62" t="s">
-        <v>1</v>
-      </c>
-      <c r="J8" s="63"/>
-      <c r="K8" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="L8" s="20" t="s">
-        <v>1</v>
+      <c r="C8" s="85"/>
+      <c r="D8" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E8" s="79" t="s">
+        <v>83</v>
+      </c>
+      <c r="F8" s="80"/>
+      <c r="G8" s="80"/>
+      <c r="H8" s="80"/>
+      <c r="I8" s="80"/>
+      <c r="J8" s="81"/>
+      <c r="K8" s="16">
+        <v>0</v>
+      </c>
+      <c r="L8" s="16">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B9" s="20">
+      <c r="B9" s="16">
         <v>12</v>
       </c>
-      <c r="C9" s="66"/>
-      <c r="D9" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E9" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="F9" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="G9" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="H9" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="I9" s="62" t="s">
-        <v>1</v>
-      </c>
-      <c r="J9" s="63"/>
-      <c r="K9" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="L9" s="20" t="s">
-        <v>1</v>
+      <c r="C9" s="85"/>
+      <c r="D9" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E9" s="79" t="s">
+        <v>83</v>
+      </c>
+      <c r="F9" s="80"/>
+      <c r="G9" s="80"/>
+      <c r="H9" s="80"/>
+      <c r="I9" s="80"/>
+      <c r="J9" s="81"/>
+      <c r="K9" s="16">
+        <v>28</v>
+      </c>
+      <c r="L9" s="16">
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="2">
         <v>13</v>
       </c>
-      <c r="C10" s="67"/>
-      <c r="D10" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I10" s="64" t="s">
-        <v>1</v>
-      </c>
-      <c r="J10" s="65"/>
-      <c r="K10" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>1</v>
+      <c r="C10" s="86"/>
+      <c r="D10" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="E10" s="73" t="s">
+        <v>84</v>
+      </c>
+      <c r="F10" s="74"/>
+      <c r="G10" s="74"/>
+      <c r="H10" s="74"/>
+      <c r="I10" s="74"/>
+      <c r="J10" s="75"/>
+      <c r="K10" s="2">
+        <v>0</v>
+      </c>
+      <c r="L10" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="2:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -2920,160 +3018,159 @@
     </row>
     <row r="12" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K12" s="22"/>
+        <v>8</v>
+      </c>
+      <c r="K12" s="18"/>
     </row>
     <row r="13" spans="2:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="75" t="s">
+      <c r="B13" s="71" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" s="72"/>
+      <c r="D13" s="72"/>
+      <c r="E13" s="72"/>
+      <c r="F13" s="91" t="s">
+        <v>58</v>
+      </c>
+      <c r="G13" s="92"/>
+      <c r="H13" s="71" t="s">
+        <v>59</v>
+      </c>
+      <c r="I13" s="72"/>
+      <c r="J13" s="72"/>
+      <c r="K13" s="72"/>
+      <c r="L13" s="101"/>
+      <c r="M13" s="106" t="s">
+        <v>60</v>
+      </c>
+      <c r="N13" s="107"/>
+    </row>
+    <row r="14" spans="2:14" ht="29.4" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="105" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="97" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="97" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="109" t="s">
+        <v>61</v>
+      </c>
+      <c r="F14" s="94" t="s">
+        <v>62</v>
+      </c>
+      <c r="G14" s="93" t="s">
+        <v>63</v>
+      </c>
+      <c r="H14" s="95" t="s">
         <v>64</v>
       </c>
-      <c r="C13" s="76"/>
-      <c r="D13" s="76"/>
-      <c r="E13" s="76"/>
-      <c r="F13" s="77" t="s">
+      <c r="I14" s="97" t="s">
+        <v>32</v>
+      </c>
+      <c r="J14" s="97" t="s">
+        <v>33</v>
+      </c>
+      <c r="K14" s="99" t="s">
+        <v>35</v>
+      </c>
+      <c r="L14" s="102" t="s">
         <v>65</v>
       </c>
-      <c r="G13" s="78"/>
-      <c r="H13" s="75" t="s">
+      <c r="M14" s="104" t="s">
         <v>66</v>
       </c>
-      <c r="I13" s="76"/>
-      <c r="J13" s="76"/>
-      <c r="K13" s="76"/>
-      <c r="L13" s="92"/>
-      <c r="M13" s="57" t="s">
+      <c r="N14" s="87" t="s">
         <v>67</v>
       </c>
-      <c r="N13" s="58"/>
-    </row>
-    <row r="14" spans="2:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="87" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" s="83" t="s">
-        <v>35</v>
-      </c>
-      <c r="D14" s="83" t="s">
-        <v>36</v>
-      </c>
-      <c r="E14" s="89" t="s">
+    </row>
+    <row r="15" spans="2:14" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="108"/>
+      <c r="C15" s="98"/>
+      <c r="D15" s="98"/>
+      <c r="E15" s="110"/>
+      <c r="F15" s="111"/>
+      <c r="G15" s="93"/>
+      <c r="H15" s="96"/>
+      <c r="I15" s="98"/>
+      <c r="J15" s="98"/>
+      <c r="K15" s="100"/>
+      <c r="L15" s="103"/>
+      <c r="M15" s="105"/>
+      <c r="N15" s="94"/>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B16" s="27">
+        <v>3</v>
+      </c>
+      <c r="C16" s="28">
+        <v>3</v>
+      </c>
+      <c r="D16" s="28">
+        <v>0</v>
+      </c>
+      <c r="E16" s="29"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="F14" s="80" t="s">
-        <v>69</v>
-      </c>
-      <c r="G14" s="79" t="s">
-        <v>70</v>
-      </c>
-      <c r="H14" s="81" t="s">
-        <v>71</v>
-      </c>
-      <c r="I14" s="83" t="s">
-        <v>34</v>
-      </c>
-      <c r="J14" s="83" t="s">
-        <v>35</v>
-      </c>
-      <c r="K14" s="85" t="s">
-        <v>37</v>
-      </c>
-      <c r="L14" s="93" t="s">
-        <v>72</v>
-      </c>
-      <c r="M14" s="95" t="s">
-        <v>73</v>
-      </c>
-      <c r="N14" s="69" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B15" s="88"/>
-      <c r="C15" s="84"/>
-      <c r="D15" s="84"/>
-      <c r="E15" s="90"/>
-      <c r="F15" s="91"/>
-      <c r="G15" s="79"/>
-      <c r="H15" s="82"/>
-      <c r="I15" s="84"/>
-      <c r="J15" s="84"/>
-      <c r="K15" s="86"/>
-      <c r="L15" s="94"/>
-      <c r="M15" s="87"/>
-      <c r="N15" s="80"/>
-    </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B16" s="31">
-        <f>SUM(C16:D16)</f>
-        <v>0</v>
-      </c>
-      <c r="C16" s="32">
-        <v>0</v>
-      </c>
-      <c r="D16" s="32">
-        <v>0</v>
-      </c>
-      <c r="E16" s="33"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="35" t="s">
-        <v>75</v>
-      </c>
-      <c r="H16" s="36" t="s">
-        <v>75</v>
-      </c>
-      <c r="I16" s="31">
+      <c r="H16" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="I16" s="27">
         <f>SUM(J16:K16)</f>
         <v>0</v>
       </c>
-      <c r="J16" s="32">
+      <c r="J16" s="28">
         <v>0</v>
       </c>
-      <c r="K16" s="37">
+      <c r="K16" s="33">
         <v>0</v>
       </c>
-      <c r="L16" s="38"/>
-      <c r="M16" s="39" t="s">
-        <v>75</v>
-      </c>
-      <c r="N16" s="40">
+      <c r="L16" s="34"/>
+      <c r="M16" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="N16" s="36">
         <f>C16</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="M13:N13"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="C14:C15"/>
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="E14:E15"/>
     <mergeCell ref="F14:F15"/>
-    <mergeCell ref="F13:G13"/>
     <mergeCell ref="G14:G15"/>
     <mergeCell ref="N14:N15"/>
     <mergeCell ref="H14:H15"/>
     <mergeCell ref="I14:I15"/>
     <mergeCell ref="K14:K15"/>
     <mergeCell ref="J14:J15"/>
-    <mergeCell ref="H13:L13"/>
     <mergeCell ref="L14:L15"/>
     <mergeCell ref="M14:M15"/>
-    <mergeCell ref="M13:N13"/>
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="B3:L3"/>
     <mergeCell ref="B4:B5"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="I5:J5"/>
     <mergeCell ref="K4:L4"/>
     <mergeCell ref="C6:C10"/>
     <mergeCell ref="E4:J4"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="D4:D5"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="I8:J8"/>
     <mergeCell ref="B13:E13"/>
+    <mergeCell ref="E5:J5"/>
+    <mergeCell ref="E6:J6"/>
+    <mergeCell ref="E7:J7"/>
+    <mergeCell ref="E8:J8"/>
+    <mergeCell ref="E9:J9"/>
+    <mergeCell ref="E10:J10"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="H13:L13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3081,6 +3178,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010058284A30843C9F43BD758DDD8294D484" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6d50638930d08c51b5585735b2be047e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="fed1744a-f275-4023-9290-77fd546fd730" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4acb07121b76573bb3c966f3dcb1b903" ns2:_="">
     <xsd:import namespace="fed1744a-f275-4023-9290-77fd546fd730"/>
@@ -3224,22 +3336,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5426D20B-58AE-4BE9-8733-DFB2BC19D8C6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6597AB9C-DC10-4824-8900-518D3B18165A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{741A764F-DFF5-4AE4-B0E7-77BD148FABB8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3255,21 +3369,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5426D20B-58AE-4BE9-8733-DFB2BC19D8C6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6597AB9C-DC10-4824-8900-518D3B18165A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
L3 Modificari, cred ca gata
</commit_message>
<xml_diff>
--- a/Docs/Lab03/Lab03_WBT_TCs_Form.xlsx
+++ b/Docs/Lab03/Lab03_WBT_TCs_Form.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28623"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3ED3188-FF8D-4DFF-8FAC-63974AE78879}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBD4BF39-DF61-41F9-98FE-A742935A9075}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="109">
   <si>
     <t>Informaţiile vor fi preluate din fişiere text.</t>
   </si>
@@ -514,6 +514,21 @@
   </si>
   <si>
     <t>l==null</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>[Payment(1, CASH, 28.0f)]</t>
+  </si>
+  <si>
+    <t>[Payment(2, CARD, 15.0f), Payment(1, CASH, 28.0f)]</t>
   </si>
 </sst>
 </file>
@@ -742,7 +757,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="37">
+  <borders count="40">
     <border>
       <left/>
       <right/>
@@ -1200,11 +1215,44 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="122">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1272,9 +1320,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1317,6 +1362,18 @@
     <xf numFmtId="0" fontId="7" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1326,18 +1383,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1377,19 +1422,37 @@
     <xf numFmtId="0" fontId="13" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1398,7 +1461,43 @@
     <xf numFmtId="0" fontId="7" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1407,113 +1506,92 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1934,12 +2012,12 @@
   <sheetData>
     <row r="1" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B1" s="7"/>
-      <c r="D1" s="43" t="s">
+      <c r="D1" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="45"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="44"/>
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B2" s="26" t="s">
@@ -1986,10 +2064,10 @@
       <c r="N7" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="O7" s="37" t="s">
+      <c r="O7" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="P7" s="38">
+      <c r="P7" s="37">
         <v>234</v>
       </c>
     </row>
@@ -2001,10 +2079,10 @@
       <c r="N8" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="O8" s="39" t="s">
+      <c r="O8" s="38" t="s">
         <v>74</v>
       </c>
-      <c r="P8" s="40">
+      <c r="P8" s="39">
         <v>234</v>
       </c>
     </row>
@@ -2018,10 +2096,10 @@
       <c r="N9" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="O9" s="41" t="s">
+      <c r="O9" s="40" t="s">
         <v>75</v>
       </c>
-      <c r="P9" s="40">
+      <c r="P9" s="39">
         <v>234</v>
       </c>
     </row>
@@ -2081,168 +2159,168 @@
   <sheetData>
     <row r="1" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B1" s="7"/>
-      <c r="D1" s="43" t="s">
+      <c r="D1" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="45"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="44"/>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B3" s="50" t="s">
+      <c r="B3" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51"/>
-      <c r="J3" s="51"/>
-      <c r="K3" s="52"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="47"/>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B6" s="43" t="s">
+      <c r="B6" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="44"/>
-      <c r="D6" s="44"/>
-      <c r="E6" s="45"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="44"/>
       <c r="F6" s="20"/>
       <c r="G6" s="20"/>
-      <c r="I6" s="43" t="s">
+      <c r="I6" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="J6" s="44"/>
-      <c r="K6" s="44"/>
-      <c r="L6" s="44"/>
-      <c r="M6" s="44"/>
-      <c r="N6" s="44"/>
-      <c r="O6" s="44"/>
-      <c r="Q6" s="43" t="s">
+      <c r="J6" s="43"/>
+      <c r="K6" s="43"/>
+      <c r="L6" s="43"/>
+      <c r="M6" s="43"/>
+      <c r="N6" s="43"/>
+      <c r="O6" s="43"/>
+      <c r="Q6" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="R6" s="44"/>
-      <c r="S6" s="44"/>
-      <c r="T6" s="44"/>
+      <c r="R6" s="43"/>
+      <c r="S6" s="43"/>
+      <c r="T6" s="43"/>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.3">
       <c r="I8" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="Q8" s="49" t="s">
+      <c r="Q8" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="R8" s="49"/>
-      <c r="S8" s="49"/>
+      <c r="R8" s="48"/>
+      <c r="S8" s="48"/>
       <c r="T8" s="22">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.3">
       <c r="I9" s="25"/>
-      <c r="Q9" s="49" t="s">
+      <c r="Q9" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="R9" s="49"/>
-      <c r="S9" s="49"/>
+      <c r="R9" s="48"/>
+      <c r="S9" s="48"/>
       <c r="T9" s="22">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="Q10" s="49" t="s">
+      <c r="Q10" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="R10" s="49" t="s">
+      <c r="R10" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="S10" s="49"/>
+      <c r="S10" s="48"/>
       <c r="T10" s="22">
         <v>5</v>
       </c>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="Q13" s="43" t="s">
+      <c r="Q13" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="R13" s="44"/>
-      <c r="S13" s="44"/>
-      <c r="T13" s="44"/>
+      <c r="R13" s="43"/>
+      <c r="S13" s="43"/>
+      <c r="T13" s="43"/>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.3">
       <c r="Q15" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="R15" s="53" t="s">
+      <c r="R15" s="52" t="s">
         <v>12</v>
       </c>
-      <c r="S15" s="54"/>
-      <c r="T15" s="55"/>
+      <c r="S15" s="53"/>
+      <c r="T15" s="54"/>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.3">
       <c r="Q16" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="R16" s="46" t="s">
+      <c r="R16" s="49" t="s">
         <v>76</v>
       </c>
-      <c r="S16" s="47"/>
-      <c r="T16" s="48"/>
+      <c r="S16" s="50"/>
+      <c r="T16" s="51"/>
     </row>
     <row r="17" spans="17:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="Q17" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="R17" s="46" t="s">
+      <c r="R17" s="49" t="s">
         <v>77</v>
       </c>
-      <c r="S17" s="47"/>
-      <c r="T17" s="48"/>
+      <c r="S17" s="50"/>
+      <c r="T17" s="51"/>
     </row>
     <row r="18" spans="17:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="Q18" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="R18" s="46" t="s">
+      <c r="R18" s="49" t="s">
         <v>81</v>
       </c>
-      <c r="S18" s="47"/>
-      <c r="T18" s="48"/>
+      <c r="S18" s="50"/>
+      <c r="T18" s="51"/>
     </row>
     <row r="19" spans="17:20" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="Q19" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="R19" s="46" t="s">
+      <c r="R19" s="49" t="s">
         <v>80</v>
       </c>
-      <c r="S19" s="47"/>
-      <c r="T19" s="48"/>
+      <c r="S19" s="50"/>
+      <c r="T19" s="51"/>
     </row>
     <row r="20" spans="17:20" x14ac:dyDescent="0.3">
       <c r="Q20" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="R20" s="46" t="s">
+      <c r="R20" s="49" t="s">
         <v>99</v>
       </c>
-      <c r="S20" s="47"/>
-      <c r="T20" s="48"/>
+      <c r="S20" s="50"/>
+      <c r="T20" s="51"/>
     </row>
     <row r="21" spans="17:20" x14ac:dyDescent="0.3">
       <c r="Q21" s="23"/>
-      <c r="R21" s="46"/>
-      <c r="S21" s="47"/>
-      <c r="T21" s="48"/>
+      <c r="R21" s="49"/>
+      <c r="S21" s="50"/>
+      <c r="T21" s="51"/>
     </row>
     <row r="24" spans="17:20" x14ac:dyDescent="0.3">
-      <c r="R24" s="46"/>
-      <c r="S24" s="47"/>
-      <c r="T24" s="48"/>
+      <c r="R24" s="49"/>
+      <c r="S24" s="50"/>
+      <c r="T24" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="17">
@@ -2251,6 +2329,11 @@
     <mergeCell ref="Q9:S9"/>
     <mergeCell ref="R16:T16"/>
     <mergeCell ref="Q13:T13"/>
+    <mergeCell ref="R19:T19"/>
+    <mergeCell ref="R17:T17"/>
+    <mergeCell ref="R15:T15"/>
+    <mergeCell ref="R21:T21"/>
+    <mergeCell ref="R20:T20"/>
     <mergeCell ref="D1:I1"/>
     <mergeCell ref="B3:K3"/>
     <mergeCell ref="Q10:S10"/>
@@ -2258,11 +2341,6 @@
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="I6:O6"/>
     <mergeCell ref="Q6:T6"/>
-    <mergeCell ref="R19:T19"/>
-    <mergeCell ref="R17:T17"/>
-    <mergeCell ref="R15:T15"/>
-    <mergeCell ref="R21:T21"/>
-    <mergeCell ref="R20:T20"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2276,10 +2354,10 @@
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="B1:AB16"/>
+  <dimension ref="B1:AC16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2307,218 +2385,224 @@
     <col min="28" max="28" width="5.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B1" s="7"/>
-      <c r="D1" s="43" t="s">
+      <c r="D1" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="45"/>
-    </row>
-    <row r="3" spans="2:28" x14ac:dyDescent="0.3">
-      <c r="B3" s="50" t="s">
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="44"/>
+    </row>
+    <row r="3" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="B3" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="52"/>
-    </row>
-    <row r="5" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="47"/>
+    </row>
+    <row r="5" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B5" s="6"/>
     </row>
-    <row r="6" spans="2:28" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B6" s="59" t="s">
+    <row r="6" spans="2:29" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B6" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="59" t="s">
+      <c r="C6" s="72" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="60" t="s">
+      <c r="D6" s="73"/>
+      <c r="E6" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="59" t="s">
+      <c r="F6" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="59"/>
-      <c r="G6" s="59"/>
-      <c r="H6" s="59"/>
-      <c r="I6" s="59"/>
-      <c r="J6" s="59"/>
-      <c r="K6" s="59"/>
-      <c r="L6" s="59"/>
-      <c r="M6" s="59"/>
-      <c r="N6" s="59"/>
-      <c r="O6" s="59"/>
-      <c r="P6" s="59"/>
-      <c r="Q6" s="59"/>
-      <c r="R6" s="59"/>
-      <c r="S6" s="59"/>
-      <c r="T6" s="59"/>
-      <c r="U6" s="59"/>
-      <c r="V6" s="59"/>
-      <c r="W6" s="59"/>
-      <c r="X6" s="59"/>
-      <c r="Y6" s="59"/>
-      <c r="Z6" s="59"/>
-      <c r="AA6" s="59"/>
-      <c r="AB6" s="59"/>
-    </row>
-    <row r="7" spans="2:28" ht="15.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="59"/>
-      <c r="C7" s="59"/>
-      <c r="D7" s="61"/>
-      <c r="E7" s="69" t="s">
+      <c r="G6" s="58"/>
+      <c r="H6" s="58"/>
+      <c r="I6" s="58"/>
+      <c r="J6" s="58"/>
+      <c r="K6" s="58"/>
+      <c r="L6" s="58"/>
+      <c r="M6" s="58"/>
+      <c r="N6" s="58"/>
+      <c r="O6" s="58"/>
+      <c r="P6" s="58"/>
+      <c r="Q6" s="58"/>
+      <c r="R6" s="58"/>
+      <c r="S6" s="58"/>
+      <c r="T6" s="58"/>
+      <c r="U6" s="58"/>
+      <c r="V6" s="58"/>
+      <c r="W6" s="58"/>
+      <c r="X6" s="58"/>
+      <c r="Y6" s="58"/>
+      <c r="Z6" s="58"/>
+      <c r="AA6" s="58"/>
+      <c r="AB6" s="58"/>
+      <c r="AC6" s="58"/>
+    </row>
+    <row r="7" spans="2:29" ht="15.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="58"/>
+      <c r="C7" s="74"/>
+      <c r="D7" s="75"/>
+      <c r="E7" s="60"/>
+      <c r="F7" s="66" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="66" t="s">
+      <c r="G7" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="G7" s="70"/>
       <c r="H7" s="70"/>
       <c r="I7" s="70"/>
       <c r="J7" s="70"/>
       <c r="K7" s="70"/>
       <c r="L7" s="70"/>
-      <c r="M7" s="67"/>
-      <c r="N7" s="56" t="s">
+      <c r="M7" s="70"/>
+      <c r="N7" s="71"/>
+      <c r="O7" s="55" t="s">
         <v>55</v>
       </c>
-      <c r="O7" s="57"/>
-      <c r="P7" s="57"/>
-      <c r="Q7" s="58"/>
-      <c r="R7" s="62" t="s">
+      <c r="P7" s="56"/>
+      <c r="Q7" s="56"/>
+      <c r="R7" s="57"/>
+      <c r="S7" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="S7" s="62"/>
-      <c r="T7" s="62"/>
-      <c r="U7" s="62"/>
-      <c r="V7" s="62"/>
-      <c r="W7" s="62"/>
-      <c r="X7" s="62"/>
-    </row>
-    <row r="8" spans="2:28" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="59"/>
-      <c r="C8" s="63" t="s">
+      <c r="T7" s="61"/>
+      <c r="U7" s="61"/>
+      <c r="V7" s="61"/>
+      <c r="W7" s="61"/>
+      <c r="X7" s="61"/>
+      <c r="Y7" s="61"/>
+    </row>
+    <row r="8" spans="2:29" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="58"/>
+      <c r="C8" s="62" t="s">
         <v>82</v>
       </c>
-      <c r="D8" s="63" t="s">
+      <c r="D8" s="59" t="s">
+        <v>104</v>
+      </c>
+      <c r="E8" s="62" t="s">
         <v>86</v>
       </c>
-      <c r="E8" s="69"/>
-      <c r="F8" s="65" t="s">
+      <c r="F8" s="67"/>
+      <c r="G8" s="64" t="s">
         <v>103</v>
       </c>
-      <c r="G8" s="65"/>
-      <c r="H8" s="65" t="s">
+      <c r="H8" s="64"/>
+      <c r="I8" s="64" t="s">
         <v>89</v>
       </c>
-      <c r="I8" s="65"/>
-      <c r="J8" s="65" t="s">
+      <c r="J8" s="64"/>
+      <c r="K8" s="64" t="s">
         <v>90</v>
       </c>
-      <c r="K8" s="65"/>
-      <c r="L8" s="66" t="s">
+      <c r="L8" s="64"/>
+      <c r="M8" s="69" t="s">
         <v>96</v>
       </c>
-      <c r="M8" s="67"/>
-      <c r="N8" s="68" t="s">
+      <c r="N8" s="71"/>
+      <c r="O8" s="65" t="s">
         <v>44</v>
       </c>
-      <c r="O8" s="68" t="s">
+      <c r="P8" s="65" t="s">
         <v>45</v>
       </c>
-      <c r="P8" s="68" t="s">
+      <c r="Q8" s="65" t="s">
         <v>47</v>
       </c>
-      <c r="Q8" s="68" t="s">
+      <c r="R8" s="65" t="s">
         <v>98</v>
       </c>
-      <c r="R8" s="62">
+      <c r="S8" s="61">
         <v>0</v>
       </c>
-      <c r="S8" s="62">
+      <c r="T8" s="61">
         <v>1</v>
       </c>
-      <c r="T8" s="62">
+      <c r="U8" s="61">
         <v>2</v>
       </c>
-      <c r="U8" s="62" t="s">
+      <c r="V8" s="61" t="s">
         <v>17</v>
       </c>
-      <c r="V8" s="62" t="s">
+      <c r="W8" s="61" t="s">
         <v>18</v>
       </c>
-      <c r="W8" s="62" t="s">
+      <c r="X8" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="X8" s="62" t="s">
+      <c r="Y8" s="61" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="2:28" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B9" s="59"/>
-      <c r="C9" s="64"/>
-      <c r="D9" s="64"/>
-      <c r="E9" s="69"/>
-      <c r="F9" s="8" t="s">
+    <row r="9" spans="2:29" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B9" s="58"/>
+      <c r="C9" s="63"/>
+      <c r="D9" s="60"/>
+      <c r="E9" s="63"/>
+      <c r="F9" s="68"/>
+      <c r="G9" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="H9" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="H9" s="8" t="s">
+      <c r="I9" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="I9" s="8" t="s">
+      <c r="J9" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="J9" s="8" t="s">
+      <c r="K9" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="K9" s="8" t="s">
+      <c r="L9" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="L9" s="8" t="s">
+      <c r="M9" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="M9" s="8" t="s">
+      <c r="N9" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="N9" s="68"/>
-      <c r="O9" s="68"/>
-      <c r="P9" s="68"/>
-      <c r="Q9" s="68"/>
-      <c r="R9" s="62"/>
-      <c r="S9" s="62"/>
-      <c r="T9" s="62"/>
-      <c r="U9" s="62"/>
-      <c r="V9" s="62"/>
-      <c r="W9" s="62"/>
-      <c r="X9" s="62"/>
-    </row>
-    <row r="10" spans="2:28" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="O9" s="65"/>
+      <c r="P9" s="65"/>
+      <c r="Q9" s="65"/>
+      <c r="R9" s="65"/>
+      <c r="S9" s="61"/>
+      <c r="T9" s="61"/>
+      <c r="U9" s="61"/>
+      <c r="V9" s="61"/>
+      <c r="W9" s="61"/>
+      <c r="X9" s="61"/>
+      <c r="Y9" s="61"/>
+    </row>
+    <row r="10" spans="2:29" ht="46.8" x14ac:dyDescent="0.3">
       <c r="B10" s="9" t="s">
         <v>42</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="E10" s="10">
         <v>28</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="F10" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12" t="s">
+      <c r="G10" s="12"/>
+      <c r="H10" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12" t="s">
-        <v>97</v>
-      </c>
+      <c r="I10" s="12"/>
       <c r="J10" s="12" t="s">
         <v>97</v>
       </c>
@@ -2528,128 +2612,137 @@
       <c r="L10" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="M10" s="12"/>
-      <c r="N10" s="13"/>
+      <c r="M10" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="N10" s="12"/>
       <c r="O10" s="13"/>
       <c r="P10" s="13"/>
-      <c r="Q10" s="13" t="s">
+      <c r="Q10" s="13"/>
+      <c r="R10" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="R10" s="14"/>
-      <c r="S10" s="14" t="s">
+      <c r="S10" s="14"/>
+      <c r="T10" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="T10" s="14"/>
       <c r="U10" s="14"/>
-      <c r="V10" s="14" t="s">
+      <c r="V10" s="14"/>
+      <c r="W10" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="W10" s="14"/>
       <c r="X10" s="14"/>
-    </row>
-    <row r="11" spans="2:28" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="Y10" s="14"/>
+    </row>
+    <row r="11" spans="2:29" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B11" s="9" t="s">
         <v>46</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E11" s="10">
         <v>0</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="F11" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12" t="s">
-        <v>97</v>
-      </c>
+      <c r="G11" s="12"/>
       <c r="H11" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="I11" s="12"/>
+      <c r="I11" s="12" t="s">
+        <v>97</v>
+      </c>
       <c r="J11" s="12"/>
       <c r="K11" s="12"/>
       <c r="L11" s="12"/>
       <c r="M11" s="12"/>
-      <c r="N11" s="13"/>
-      <c r="O11" s="13" t="s">
+      <c r="N11" s="12"/>
+      <c r="O11" s="13"/>
+      <c r="P11" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="P11" s="13"/>
       <c r="Q11" s="13"/>
-      <c r="R11" s="14" t="s">
+      <c r="R11" s="13"/>
+      <c r="S11" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="S11" s="14"/>
       <c r="T11" s="14"/>
       <c r="U11" s="14"/>
       <c r="V11" s="14"/>
       <c r="W11" s="14"/>
       <c r="X11" s="14"/>
-    </row>
-    <row r="12" spans="2:28" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="Y11" s="14"/>
+    </row>
+    <row r="12" spans="2:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B12" s="9" t="s">
         <v>85</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="D12" s="42">
+      <c r="D12" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="E12" s="41">
         <v>0</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="F12" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="F12" s="12" t="s">
+      <c r="G12" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="G12" s="12"/>
       <c r="H12" s="12"/>
-      <c r="I12" s="12" t="s">
+      <c r="I12" s="12"/>
+      <c r="J12" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="J12" s="12"/>
       <c r="K12" s="12"/>
       <c r="L12" s="12"/>
       <c r="M12" s="12"/>
-      <c r="N12" s="13" t="s">
+      <c r="N12" s="12"/>
+      <c r="O12" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="O12" s="13"/>
       <c r="P12" s="13"/>
       <c r="Q12" s="13"/>
-      <c r="R12" s="14" t="s">
+      <c r="R12" s="13"/>
+      <c r="S12" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="S12" s="14"/>
       <c r="T12" s="14"/>
       <c r="U12" s="14"/>
       <c r="V12" s="14"/>
       <c r="W12" s="14"/>
       <c r="X12" s="14"/>
-    </row>
-    <row r="13" spans="2:28" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="Y12" s="14"/>
+    </row>
+    <row r="13" spans="2:29" ht="62.4" x14ac:dyDescent="0.3">
       <c r="B13" s="9" t="s">
         <v>87</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="E13" s="10">
         <v>28</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="F13" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12" t="s">
+      <c r="G13" s="12"/>
+      <c r="H13" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12" t="s">
-        <v>97</v>
-      </c>
+      <c r="I13" s="12"/>
       <c r="J13" s="12" t="s">
         <v>97</v>
       </c>
@@ -2662,81 +2755,87 @@
       <c r="M13" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="N13" s="13"/>
+      <c r="N13" s="12" t="s">
+        <v>97</v>
+      </c>
       <c r="O13" s="13"/>
-      <c r="P13" s="13" t="s">
-        <v>97</v>
-      </c>
+      <c r="P13" s="13"/>
       <c r="Q13" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="R13" s="14"/>
+      <c r="R13" s="13" t="s">
+        <v>97</v>
+      </c>
       <c r="S13" s="14"/>
       <c r="T13" s="14"/>
       <c r="U13" s="14"/>
-      <c r="V13" s="14" t="s">
+      <c r="V13" s="14"/>
+      <c r="W13" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="W13" s="14"/>
       <c r="X13" s="14"/>
-    </row>
-    <row r="14" spans="2:28" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="Y13" s="14"/>
+    </row>
+    <row r="14" spans="2:29" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B14" s="9" t="s">
         <v>88</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="D14" s="10">
+      <c r="D14" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="E14" s="10">
         <v>0</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="F14" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12" t="s">
+      <c r="G14" s="12"/>
+      <c r="H14" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12" t="s">
-        <v>97</v>
-      </c>
+      <c r="I14" s="12"/>
       <c r="J14" s="12" t="s">
         <v>97</v>
       </c>
       <c r="K14" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="L14" s="12"/>
-      <c r="M14" s="12" t="s">
+      <c r="L14" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="N14" s="13"/>
+      <c r="M14" s="12"/>
+      <c r="N14" s="12" t="s">
+        <v>97</v>
+      </c>
       <c r="O14" s="13"/>
-      <c r="P14" s="13" t="s">
+      <c r="P14" s="13"/>
+      <c r="Q14" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="Q14" s="13"/>
-      <c r="R14" s="14"/>
-      <c r="S14" s="14" t="s">
+      <c r="R14" s="13"/>
+      <c r="S14" s="14"/>
+      <c r="T14" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="T14" s="14"/>
       <c r="U14" s="14"/>
-      <c r="V14" s="14" t="s">
+      <c r="V14" s="14"/>
+      <c r="W14" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="W14" s="14"/>
       <c r="X14" s="14"/>
-    </row>
-    <row r="15" spans="2:28" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="Y14" s="14"/>
+    </row>
+    <row r="15" spans="2:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B15" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C15" s="9"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="12"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="11"/>
       <c r="G15" s="12"/>
       <c r="H15" s="12"/>
       <c r="I15" s="12"/>
@@ -2744,50 +2843,52 @@
       <c r="K15" s="12"/>
       <c r="L15" s="12"/>
       <c r="M15" s="12"/>
-      <c r="N15" s="13"/>
+      <c r="N15" s="12"/>
       <c r="O15" s="13"/>
       <c r="P15" s="13"/>
       <c r="Q15" s="13"/>
-      <c r="R15" s="14"/>
+      <c r="R15" s="13"/>
       <c r="S15" s="14"/>
       <c r="T15" s="14"/>
       <c r="U15" s="14"/>
       <c r="V15" s="14"/>
       <c r="W15" s="14"/>
       <c r="X15" s="14"/>
-    </row>
-    <row r="16" spans="2:28" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="Y15" s="14"/>
+    </row>
+    <row r="16" spans="2:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B16" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="27">
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="E7:E9"/>
-    <mergeCell ref="F7:M7"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="R8:R9"/>
-    <mergeCell ref="N8:N9"/>
+  <mergeCells count="28">
     <mergeCell ref="O8:O9"/>
     <mergeCell ref="P8:P9"/>
     <mergeCell ref="Q8:Q9"/>
-    <mergeCell ref="N7:Q7"/>
+    <mergeCell ref="R8:R9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="G7:N7"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="C6:D7"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="O7:R7"/>
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="B6:B9"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:AB6"/>
-    <mergeCell ref="V8:V9"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:AC6"/>
     <mergeCell ref="W8:W9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="S8:S9"/>
+    <mergeCell ref="X8:X9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="G8:H8"/>
     <mergeCell ref="T8:T9"/>
     <mergeCell ref="U8:U9"/>
-    <mergeCell ref="R7:X7"/>
-    <mergeCell ref="X8:X9"/>
+    <mergeCell ref="V8:V9"/>
+    <mergeCell ref="S7:Y7"/>
+    <mergeCell ref="Y8:Y9"/>
+    <mergeCell ref="S8:S9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2802,7 +2903,7 @@
   <dimension ref="B1:N16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2811,7 +2912,7 @@
     <col min="4" max="4" width="11.21875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.44140625" customWidth="1"/>
     <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.21875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.109375" bestFit="1" customWidth="1"/>
@@ -2822,30 +2923,30 @@
   <sheetData>
     <row r="1" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B1" s="7"/>
-      <c r="D1" s="43" t="s">
+      <c r="D1" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="45"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="44"/>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B3" s="82" t="s">
+      <c r="B3" s="79" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="82"/>
-      <c r="D3" s="82"/>
-      <c r="E3" s="82"/>
-      <c r="F3" s="82"/>
-      <c r="G3" s="82"/>
-      <c r="H3" s="82"/>
-      <c r="I3" s="82"/>
-      <c r="J3" s="82"/>
-      <c r="K3" s="82"/>
-      <c r="L3" s="82"/>
+      <c r="C3" s="79"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="79"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="79"/>
+      <c r="H3" s="79"/>
+      <c r="I3" s="79"/>
+      <c r="J3" s="79"/>
+      <c r="K3" s="79"/>
+      <c r="L3" s="79"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B4" s="83" t="s">
+      <c r="B4" s="80" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="87" t="s">
@@ -2854,31 +2955,33 @@
       <c r="D4" s="89" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="79" t="s">
+      <c r="E4" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="80"/>
-      <c r="G4" s="80"/>
-      <c r="H4" s="80"/>
-      <c r="I4" s="80"/>
-      <c r="J4" s="81"/>
-      <c r="K4" s="79" t="s">
+      <c r="F4" s="86"/>
+      <c r="G4" s="86"/>
+      <c r="H4" s="86"/>
+      <c r="I4" s="86"/>
+      <c r="J4" s="83"/>
+      <c r="K4" s="82" t="s">
         <v>3</v>
       </c>
-      <c r="L4" s="81"/>
+      <c r="L4" s="83"/>
     </row>
     <row r="5" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="84"/>
+      <c r="B5" s="81"/>
       <c r="C5" s="88"/>
       <c r="D5" s="90"/>
-      <c r="E5" s="73" t="s">
+      <c r="E5" s="115" t="s">
         <v>82</v>
       </c>
-      <c r="F5" s="74"/>
-      <c r="G5" s="74"/>
-      <c r="H5" s="74"/>
-      <c r="I5" s="74"/>
-      <c r="J5" s="75"/>
+      <c r="F5" s="116"/>
+      <c r="G5" s="91" t="s">
+        <v>104</v>
+      </c>
+      <c r="H5" s="91"/>
+      <c r="I5" s="91"/>
+      <c r="J5" s="92"/>
       <c r="K5" s="2" t="s">
         <v>4</v>
       </c>
@@ -2890,20 +2993,22 @@
       <c r="B6" s="16">
         <v>9</v>
       </c>
-      <c r="C6" s="85" t="s">
+      <c r="C6" s="84" t="s">
         <v>36</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E6" s="76" t="s">
+      <c r="E6" s="117" t="s">
         <v>83</v>
       </c>
-      <c r="F6" s="77"/>
-      <c r="G6" s="77"/>
-      <c r="H6" s="77"/>
-      <c r="I6" s="77"/>
-      <c r="J6" s="78"/>
+      <c r="F6" s="118"/>
+      <c r="G6" s="93" t="s">
+        <v>107</v>
+      </c>
+      <c r="H6" s="93"/>
+      <c r="I6" s="93"/>
+      <c r="J6" s="94"/>
       <c r="K6" s="17">
         <v>28</v>
       </c>
@@ -2915,18 +3020,20 @@
       <c r="B7" s="16">
         <v>10</v>
       </c>
-      <c r="C7" s="85"/>
+      <c r="C7" s="84"/>
       <c r="D7" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="E7" s="79" t="s">
+      <c r="E7" s="119" t="s">
         <v>83</v>
       </c>
-      <c r="F7" s="80"/>
-      <c r="G7" s="80"/>
-      <c r="H7" s="80"/>
-      <c r="I7" s="80"/>
-      <c r="J7" s="81"/>
+      <c r="F7" s="120"/>
+      <c r="G7" s="86" t="s">
+        <v>105</v>
+      </c>
+      <c r="H7" s="86"/>
+      <c r="I7" s="86"/>
+      <c r="J7" s="83"/>
       <c r="K7" s="16">
         <v>0</v>
       </c>
@@ -2938,18 +3045,20 @@
       <c r="B8" s="16">
         <v>11</v>
       </c>
-      <c r="C8" s="85"/>
+      <c r="C8" s="84"/>
       <c r="D8" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="E8" s="79" t="s">
+      <c r="E8" s="119" t="s">
         <v>83</v>
       </c>
-      <c r="F8" s="80"/>
-      <c r="G8" s="80"/>
-      <c r="H8" s="80"/>
-      <c r="I8" s="80"/>
-      <c r="J8" s="81"/>
+      <c r="F8" s="120"/>
+      <c r="G8" s="86" t="s">
+        <v>106</v>
+      </c>
+      <c r="H8" s="86"/>
+      <c r="I8" s="86"/>
+      <c r="J8" s="83"/>
       <c r="K8" s="16">
         <v>0</v>
       </c>
@@ -2961,18 +3070,20 @@
       <c r="B9" s="16">
         <v>12</v>
       </c>
-      <c r="C9" s="85"/>
+      <c r="C9" s="84"/>
       <c r="D9" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="E9" s="79" t="s">
+      <c r="E9" s="119" t="s">
         <v>83</v>
       </c>
-      <c r="F9" s="80"/>
-      <c r="G9" s="80"/>
-      <c r="H9" s="80"/>
-      <c r="I9" s="80"/>
-      <c r="J9" s="81"/>
+      <c r="F9" s="120"/>
+      <c r="G9" s="86" t="s">
+        <v>108</v>
+      </c>
+      <c r="H9" s="86"/>
+      <c r="I9" s="86"/>
+      <c r="J9" s="83"/>
       <c r="K9" s="16">
         <v>28</v>
       </c>
@@ -2984,18 +3095,20 @@
       <c r="B10" s="2">
         <v>13</v>
       </c>
-      <c r="C10" s="86"/>
+      <c r="C10" s="85"/>
       <c r="D10" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="E10" s="73" t="s">
+      <c r="E10" s="115" t="s">
         <v>84</v>
       </c>
-      <c r="F10" s="74"/>
-      <c r="G10" s="74"/>
-      <c r="H10" s="74"/>
-      <c r="I10" s="74"/>
-      <c r="J10" s="75"/>
+      <c r="F10" s="116"/>
+      <c r="G10" s="91" t="s">
+        <v>107</v>
+      </c>
+      <c r="H10" s="91"/>
+      <c r="I10" s="91"/>
+      <c r="J10" s="92"/>
       <c r="K10" s="2">
         <v>0</v>
       </c>
@@ -3023,63 +3136,63 @@
       <c r="K12" s="18"/>
     </row>
     <row r="13" spans="2:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="71" t="s">
+      <c r="B13" s="76" t="s">
         <v>57</v>
       </c>
-      <c r="C13" s="72"/>
-      <c r="D13" s="72"/>
-      <c r="E13" s="72"/>
-      <c r="F13" s="91" t="s">
+      <c r="C13" s="77"/>
+      <c r="D13" s="77"/>
+      <c r="E13" s="77"/>
+      <c r="F13" s="113" t="s">
         <v>58</v>
       </c>
-      <c r="G13" s="92"/>
-      <c r="H13" s="71" t="s">
+      <c r="G13" s="114"/>
+      <c r="H13" s="76" t="s">
         <v>59</v>
       </c>
-      <c r="I13" s="72"/>
-      <c r="J13" s="72"/>
-      <c r="K13" s="72"/>
-      <c r="L13" s="101"/>
-      <c r="M13" s="106" t="s">
+      <c r="I13" s="77"/>
+      <c r="J13" s="77"/>
+      <c r="K13" s="77"/>
+      <c r="L13" s="78"/>
+      <c r="M13" s="95" t="s">
         <v>60</v>
       </c>
-      <c r="N13" s="107"/>
+      <c r="N13" s="96"/>
     </row>
     <row r="14" spans="2:14" ht="29.4" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="105" t="s">
+      <c r="B14" s="97" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="97" t="s">
+      <c r="C14" s="99" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="97" t="s">
+      <c r="D14" s="99" t="s">
         <v>34</v>
       </c>
-      <c r="E14" s="109" t="s">
+      <c r="E14" s="101" t="s">
         <v>61</v>
       </c>
-      <c r="F14" s="94" t="s">
+      <c r="F14" s="103" t="s">
         <v>62</v>
       </c>
-      <c r="G14" s="93" t="s">
+      <c r="G14" s="105" t="s">
         <v>63</v>
       </c>
-      <c r="H14" s="95" t="s">
+      <c r="H14" s="106" t="s">
         <v>64</v>
       </c>
-      <c r="I14" s="97" t="s">
+      <c r="I14" s="99" t="s">
         <v>32</v>
       </c>
-      <c r="J14" s="97" t="s">
+      <c r="J14" s="99" t="s">
         <v>33</v>
       </c>
-      <c r="K14" s="99" t="s">
+      <c r="K14" s="108" t="s">
         <v>35</v>
       </c>
-      <c r="L14" s="102" t="s">
+      <c r="L14" s="110" t="s">
         <v>65</v>
       </c>
-      <c r="M14" s="104" t="s">
+      <c r="M14" s="112" t="s">
         <v>66</v>
       </c>
       <c r="N14" s="87" t="s">
@@ -3087,19 +3200,19 @@
       </c>
     </row>
     <row r="15" spans="2:14" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="108"/>
-      <c r="C15" s="98"/>
-      <c r="D15" s="98"/>
-      <c r="E15" s="110"/>
-      <c r="F15" s="111"/>
-      <c r="G15" s="93"/>
-      <c r="H15" s="96"/>
-      <c r="I15" s="98"/>
-      <c r="J15" s="98"/>
-      <c r="K15" s="100"/>
-      <c r="L15" s="103"/>
-      <c r="M15" s="105"/>
-      <c r="N15" s="94"/>
+      <c r="B15" s="98"/>
+      <c r="C15" s="100"/>
+      <c r="D15" s="100"/>
+      <c r="E15" s="102"/>
+      <c r="F15" s="104"/>
+      <c r="G15" s="105"/>
+      <c r="H15" s="107"/>
+      <c r="I15" s="100"/>
+      <c r="J15" s="100"/>
+      <c r="K15" s="109"/>
+      <c r="L15" s="111"/>
+      <c r="M15" s="97"/>
+      <c r="N15" s="103"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B16" s="27">
@@ -3111,12 +3224,14 @@
       <c r="D16" s="28">
         <v>0</v>
       </c>
-      <c r="E16" s="29"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="31" t="s">
+      <c r="E16" s="121">
+        <v>1</v>
+      </c>
+      <c r="F16" s="29"/>
+      <c r="G16" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="H16" s="32" t="s">
+      <c r="H16" s="31" t="s">
         <v>68</v>
       </c>
       <c r="I16" s="27">
@@ -3126,20 +3241,26 @@
       <c r="J16" s="28">
         <v>0</v>
       </c>
-      <c r="K16" s="33">
+      <c r="K16" s="32">
         <v>0</v>
       </c>
-      <c r="L16" s="34"/>
-      <c r="M16" s="35" t="s">
+      <c r="L16" s="33"/>
+      <c r="M16" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="N16" s="36">
+      <c r="N16" s="35">
         <f>C16</f>
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="G10:J10"/>
+    <mergeCell ref="G5:J5"/>
+    <mergeCell ref="G6:J6"/>
+    <mergeCell ref="G7:J7"/>
+    <mergeCell ref="G8:J8"/>
+    <mergeCell ref="G9:J9"/>
     <mergeCell ref="M13:N13"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="C14:C15"/>
@@ -3154,6 +3275,9 @@
     <mergeCell ref="J14:J15"/>
     <mergeCell ref="L14:L15"/>
     <mergeCell ref="M14:M15"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="H13:L13"/>
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="B3:L3"/>
     <mergeCell ref="B4:B5"/>
@@ -3162,15 +3286,6 @@
     <mergeCell ref="E4:J4"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="D4:D5"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="E5:J5"/>
-    <mergeCell ref="E6:J6"/>
-    <mergeCell ref="E7:J7"/>
-    <mergeCell ref="E8:J8"/>
-    <mergeCell ref="E9:J9"/>
-    <mergeCell ref="E10:J10"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="H13:L13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3178,21 +3293,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010058284A30843C9F43BD758DDD8294D484" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6d50638930d08c51b5585735b2be047e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="fed1744a-f275-4023-9290-77fd546fd730" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4acb07121b76573bb3c966f3dcb1b903" ns2:_="">
     <xsd:import namespace="fed1744a-f275-4023-9290-77fd546fd730"/>
@@ -3336,24 +3436,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5426D20B-58AE-4BE9-8733-DFB2BC19D8C6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6597AB9C-DC10-4824-8900-518D3B18165A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{741A764F-DFF5-4AE4-B0E7-77BD148FABB8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3369,4 +3467,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5426D20B-58AE-4BE9-8733-DFB2BC19D8C6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6597AB9C-DC10-4824-8900-518D3B18165A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>